<commit_message>
[12.0][FIX] escape char in excel
</commit_message>
<xml_diff>
--- a/altinkaya_excel_export/export_account_payment_xlsx/payments.xlsx
+++ b/altinkaya_excel_export/export_account_payment_xlsx/payments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">Tarih</t>
   </si>
@@ -37,19 +37,16 @@
     <t xml:space="preserve">Vergi No</t>
   </si>
   <si>
-    <t xml:space="preserve">Toplam</t>
-  </si>
-  <si>
     <t xml:space="preserve">Muhasebe Kodu</t>
   </si>
   <si>
     <t xml:space="preserve">Çek no</t>
   </si>
   <si>
-    <t xml:space="preserve">Para birim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para birimi tutarı</t>
+    <t xml:space="preserve">Para birimi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para Birimi Tutarı</t>
   </si>
 </sst>
 </file>
@@ -182,19 +179,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:HT1"/>
+  <dimension ref="A1:HS1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -217,20 +215,18 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -447,7 +443,6 @@
       <c r="HQ1" s="4"/>
       <c r="HR1" s="4"/>
       <c r="HS1" s="4"/>
-      <c r="HT1" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>